<commit_message>
Added SpringAhead and Deltek rates
</commit_message>
<xml_diff>
--- a/BLU_ET_2020_0927_Projection.xlsx
+++ b/BLU_ET_2020_0927_Projection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://belcan-my.sharepoint.com/personal/jtreptow_belcan_com/Documents/BlueOrigin/2020_Base2_Personel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://belcan-my.sharepoint.com/personal/jtreptow_belcan_com/Documents/BlueOrigin/2020_Base2_Personel/ConsultantTimeReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{025CEDEC-16A1-4366-B657-1CD2174ED357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_2DAE8219C56EC8DE671498B7575DCE3AB749C6CB" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55A694AA-6C89-4718-84CC-6ED7AC7D6AEA}"/>
   <bookViews>
-    <workbookView xWindow="-36930" yWindow="710" windowWidth="35460" windowHeight="18590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37520" yWindow="540" windowWidth="36450" windowHeight="18590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BudgetProjection" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -378,13 +378,29 @@
   </si>
   <si>
     <t>Weekly Dollar Total</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Projected Year Totals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year To Date </t>
+  </si>
+  <si>
+    <t>Estimate To Complete (ETC)</t>
+  </si>
+  <si>
+    <t>Estimate At Complete (EAC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -417,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -426,6 +442,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,9 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG40"/>
+  <dimension ref="A1:BG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1110,8 +1129,8 @@
         <v>992.4249999999995</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F38" si="2">B3 * E3</f>
-        <v>214363.7999999999</v>
+        <f t="shared" ref="F3:F38" si="2">SUM(B3*G3,B3*H3,B3*I3,B3*J3,B3*K3,B3*L3,B3*M3,B3*N3,B3*O3,B3*P3,B3*Q3,B3*R3,B3*S3,B3*T3,B3*U3,B3*V3,B3*W3,B3*X3,B3*Y3,B3*Z3,B3*AA3,B3*AB3,B3*AC3,B3*AD3,B3*AE3,B3*AF3,B3*AG3,B3*AH3,B3*AI3,B3*AJ3,B3*AK3,C3*AL3,C3*AM3,C3*AN3,C3*AO3,C3*AP3,C3*AQ3,C3*AR3,C3*AS3,C3*AT3,C3*AU3,C3*AV3,C3*AW3,C3*AX3,C3*AY3,C3*AZ3,C3*BA3,C3*BB3,C3*BC3,C3*BD3,C3*BE3,C3*BF3,C3*BG3)</f>
+        <v>214363.79999999987</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -1699,7 +1718,7 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>298076.24347826076</v>
+        <v>298076.24347826093</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -1895,7 +1914,7 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>119016</v>
+        <v>121446</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -2091,7 +2110,7 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>171115.78421052636</v>
+        <v>171115.78421052627</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2483,7 +2502,7 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>11808.749999999996</v>
+        <v>11808.75</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -2875,7 +2894,7 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>361981.69411764678</v>
+        <v>361981.6941176473</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -3267,7 +3286,7 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>328180.8000000001</v>
+        <v>328180.79999999993</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
@@ -3463,7 +3482,7 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>172931.0476190476</v>
+        <v>172931.04761904757</v>
       </c>
       <c r="G15" s="4">
         <v>0</v>
@@ -3659,7 +3678,7 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>368226.94230769214</v>
+        <v>368226.9423076922</v>
       </c>
       <c r="G16" s="4">
         <v>15</v>
@@ -3855,7 +3874,7 @@
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>250695.50000000006</v>
+        <v>250695.5</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
@@ -4051,7 +4070,7 @@
       </c>
       <c r="F18" s="5">
         <f t="shared" si="2"/>
-        <v>441052.74324324314</v>
+        <v>441052.7432432432</v>
       </c>
       <c r="G18" s="4">
         <v>0</v>
@@ -4247,7 +4266,7 @@
       </c>
       <c r="F19" s="5">
         <f t="shared" si="2"/>
-        <v>286856.3076923078</v>
+        <v>286856.30769230775</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -4443,7 +4462,7 @@
       </c>
       <c r="F20" s="5">
         <f t="shared" si="2"/>
-        <v>289752.92307692301</v>
+        <v>289752.92307692312</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -4835,7 +4854,7 @@
       </c>
       <c r="F22" s="5">
         <f t="shared" si="2"/>
-        <v>238519.90588235305</v>
+        <v>238519.90588235296</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
@@ -5031,7 +5050,7 @@
       </c>
       <c r="F23" s="5">
         <f t="shared" si="2"/>
-        <v>336725.37931034504</v>
+        <v>336725.37931034487</v>
       </c>
       <c r="G23" s="4">
         <v>0</v>
@@ -5227,7 +5246,7 @@
       </c>
       <c r="F24" s="5">
         <f t="shared" si="2"/>
-        <v>372162.10909090895</v>
+        <v>372162.10909090936</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -5423,7 +5442,7 @@
       </c>
       <c r="F25" s="5">
         <f t="shared" si="2"/>
-        <v>333503.64705882379</v>
+        <v>333503.64705882367</v>
       </c>
       <c r="G25" s="4">
         <v>0</v>
@@ -5619,7 +5638,7 @@
       </c>
       <c r="F26" s="5">
         <f t="shared" si="2"/>
-        <v>394369.2972972971</v>
+        <v>394369.29729729745</v>
       </c>
       <c r="G26" s="4">
         <v>0</v>
@@ -5815,7 +5834,7 @@
       </c>
       <c r="F27" s="5">
         <f t="shared" si="2"/>
-        <v>259964.63999999984</v>
+        <v>259964.63999999987</v>
       </c>
       <c r="G27" s="4">
         <v>0</v>
@@ -6011,7 +6030,7 @@
       </c>
       <c r="F28" s="5">
         <f t="shared" si="2"/>
-        <v>374037.11999999994</v>
+        <v>374037.12000000023</v>
       </c>
       <c r="G28" s="4">
         <v>0</v>
@@ -6795,7 +6814,7 @@
       </c>
       <c r="F32" s="5">
         <f t="shared" si="2"/>
-        <v>394182.69230769202</v>
+        <v>394182.6923076926</v>
       </c>
       <c r="G32" s="4">
         <v>16</v>
@@ -7187,7 +7206,7 @@
       </c>
       <c r="F34" s="5">
         <f t="shared" si="2"/>
-        <v>233041.0800000001</v>
+        <v>233041.08000000007</v>
       </c>
       <c r="G34" s="4">
         <v>0</v>
@@ -7577,7 +7596,7 @@
       </c>
       <c r="F36" s="5">
         <f t="shared" si="2"/>
-        <v>338772.99999999983</v>
+        <v>338773</v>
       </c>
       <c r="G36" s="4">
         <v>0</v>
@@ -7773,7 +7792,7 @@
       </c>
       <c r="F37" s="5">
         <f t="shared" si="2"/>
-        <v>128059.2083333333</v>
+        <v>128059.20833333336</v>
       </c>
       <c r="G37" s="4">
         <v>0</v>
@@ -8153,8 +8172,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4">
-        <f>SUM(E3:E38)</f>
-        <v>41930.956790606921</v>
+        <v>41930.956790606797</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="4">
@@ -8379,8 +8397,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
       <c r="F40" s="5">
-        <f>SUM(F3:F38)</f>
-        <v>8776115.5432872716</v>
+        <v>8776115.5432872735</v>
       </c>
       <c r="G40" s="5">
         <f>SUM(B3*G3,B4*G4,B5*G5,B6*G6,B7*G7,B8*G8,B9*G9,B10*G10,B11*G11,B12*G12,B13*G13,B14*G14,B15*G15,B16*G16,B17*G17,B18*G18,B19*G19,B20*G20,B21*G21,B22*G22,B23*G23,B24*G24,B25*G25,B26*G26,B27*G27,B28*G28,B29*G29,B30*G30,B31*G31,B32*G32,B33*G33,B34*G34,B35*G35,B36*G36,B37*G37,B38*G38)</f>
@@ -8595,7 +8612,56 @@
         <v>83566.373981030643</v>
       </c>
     </row>
+    <row r="41" spans="1:59" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="6">
+        <v>8958790</v>
+      </c>
+    </row>
+    <row r="42" spans="1:59" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42">
+        <f>SUM(E3:E38)</f>
+        <v>41930.956790606921</v>
+      </c>
+      <c r="F42" s="5">
+        <f>SUM(F3:F38)</f>
+        <v>8778545.5432872716</v>
+      </c>
+    </row>
+    <row r="43" spans="1:59" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="5">
+        <f>SUM(G40:AS40)</f>
+        <v>6255406.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:59" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="5">
+        <f>F41-F43</f>
+        <v>2703383.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:59" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="5">
+        <f>F41-F42</f>
+        <v>180244.45671272837</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Total summary data formulas, sorting and sticky headers
</commit_message>
<xml_diff>
--- a/BLU_ET_2020_0927_Projection.xlsx
+++ b/BLU_ET_2020_0927_Projection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://belcan-my.sharepoint.com/personal/jtreptow_belcan_com/Documents/BlueOrigin/2020_Base2_Personel/ConsultantTimeReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_2DAE8219C56EC8DE671498B7575DCE3AB749C6CB" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55A694AA-6C89-4718-84CC-6ED7AC7D6AEA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{C8B88995-7AAE-44C7-B4BA-3BF64274F6A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37520" yWindow="540" windowWidth="36450" windowHeight="18590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Rate</t>
+    <t>SA Rate</t>
   </si>
   <si>
     <t>Deltek Rate</t>
@@ -374,10 +374,10 @@
     <t>Nguyen, Quang-Huy</t>
   </si>
   <si>
-    <t>Weekly Hour Total</t>
-  </si>
-  <si>
-    <t>Weekly Dollar Total</t>
+    <t>Hours Total/Week</t>
+  </si>
+  <si>
+    <t>Dollars Total/Week</t>
   </si>
   <si>
     <t>Budget</t>
@@ -399,8 +399,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -433,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -442,7 +441,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,14 +746,16 @@
   <dimension ref="A1:BG45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -7990,176 +7990,176 @@
         <f t="shared" si="2"/>
         <v>104880</v>
       </c>
-      <c r="G38" s="4">
-        <v>0</v>
-      </c>
-      <c r="H38" s="4">
-        <v>0</v>
-      </c>
-      <c r="I38" s="4">
-        <v>0</v>
-      </c>
-      <c r="J38" s="4">
-        <v>0</v>
-      </c>
-      <c r="K38" s="4">
-        <v>0</v>
-      </c>
-      <c r="L38" s="4">
-        <v>0</v>
-      </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
-        <v>0</v>
-      </c>
-      <c r="O38" s="4">
-        <v>0</v>
-      </c>
-      <c r="P38" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="4">
-        <v>0</v>
-      </c>
-      <c r="R38" s="4">
-        <v>0</v>
-      </c>
-      <c r="S38" s="4">
-        <v>0</v>
-      </c>
-      <c r="T38" s="4">
-        <v>0</v>
-      </c>
-      <c r="U38" s="4">
-        <v>0</v>
-      </c>
-      <c r="V38" s="4">
-        <v>0</v>
-      </c>
-      <c r="W38" s="4">
-        <v>0</v>
-      </c>
-      <c r="X38" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK38" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL38" s="4">
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
+        <v>0</v>
+      </c>
+      <c r="K38" s="5">
+        <v>0</v>
+      </c>
+      <c r="L38" s="5">
+        <v>0</v>
+      </c>
+      <c r="M38" s="5">
+        <v>0</v>
+      </c>
+      <c r="N38" s="5">
+        <v>0</v>
+      </c>
+      <c r="O38" s="5">
+        <v>0</v>
+      </c>
+      <c r="P38" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>0</v>
+      </c>
+      <c r="R38" s="5">
+        <v>0</v>
+      </c>
+      <c r="S38" s="5">
+        <v>0</v>
+      </c>
+      <c r="T38" s="5">
+        <v>0</v>
+      </c>
+      <c r="U38" s="5">
+        <v>0</v>
+      </c>
+      <c r="V38" s="5">
+        <v>0</v>
+      </c>
+      <c r="W38" s="5">
+        <v>0</v>
+      </c>
+      <c r="X38" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="5">
         <v>36</v>
       </c>
-      <c r="AM38" s="4">
+      <c r="AM38" s="5">
         <v>39</v>
       </c>
-      <c r="AN38" s="4">
-        <v>40</v>
-      </c>
-      <c r="AO38" s="4">
-        <v>40</v>
-      </c>
-      <c r="AP38" s="4">
+      <c r="AN38" s="5">
+        <v>40</v>
+      </c>
+      <c r="AO38" s="5">
+        <v>40</v>
+      </c>
+      <c r="AP38" s="5">
         <v>26</v>
       </c>
-      <c r="AQ38" s="4">
+      <c r="AQ38" s="5">
         <v>2</v>
       </c>
-      <c r="AR38" s="4">
+      <c r="AR38" s="5">
         <v>7</v>
       </c>
-      <c r="AS38" s="4">
+      <c r="AS38" s="5">
         <v>22</v>
       </c>
-      <c r="AT38" s="4">
+      <c r="AT38" s="5">
         <f>IF((40 - (40 - $AT$2)) &lt; 0, 0,(40 - (40 - $AT$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="AU38" s="4">
+      <c r="AU38" s="5">
         <f>IF((40 - (40 - $AU$2)) &lt; 0, 0,(40 - (40 - $AU$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="AV38" s="4">
+      <c r="AV38" s="5">
         <f>IF((40 - (40 - $AV$2)) &lt; 0, 0,(40 - (40 - $AV$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="AW38" s="4">
+      <c r="AW38" s="5">
         <f>IF((40 - (40 - $AW$2)) &lt; 0, 0,(40 - (40 - $AW$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="AX38" s="4">
+      <c r="AX38" s="5">
         <f>IF((40 - (40 - $AX$2)) &lt; 0, 0,(40 - (40 - $AX$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="AY38" s="4">
+      <c r="AY38" s="5">
         <f>IF((40 - (40 - $AY$2)) &lt; 0, 0,(40 - (40 - $AY$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="AZ38" s="4">
+      <c r="AZ38" s="5">
         <f>IF((40 - (40 - $AZ$2)) &lt; 0, 0,(40 - (40 - $AZ$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="BA38" s="4">
+      <c r="BA38" s="5">
         <f>IF((40 - (40 - $BA$2)) &lt; 0, 0,(40 - (40 - $BA$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="BB38" s="4">
+      <c r="BB38" s="5">
         <f>IF((40 - (40 - $BB$2)) &lt; 0, 0,(40 - (40 - $BB$2)) * D38)</f>
         <v>15.9375</v>
       </c>
-      <c r="BC38" s="4">
+      <c r="BC38" s="5">
         <f>IF((40 - (40 - $BC$2)) &lt; 0, 0,(40 - (40 - $BC$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="BD38" s="4">
+      <c r="BD38" s="5">
         <f>IF((40 - (40 - $BD$2)) &lt; 0, 0,(40 - (40 - $BD$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="BE38" s="4">
+      <c r="BE38" s="5">
         <f>IF((40 - (40 - $BE$2)) &lt; 0, 0,(40 - (40 - $BE$2)) * D38)</f>
         <v>26.5625</v>
       </c>
-      <c r="BF38" s="4">
+      <c r="BF38" s="5">
         <f>IF((40 - (40 - $BF$2)) &lt; 0, 0,(40 - (40 - $BF$2)) * D38)</f>
         <v>15.9375</v>
       </c>
-      <c r="BG38" s="4">
+      <c r="BG38" s="5">
         <f>IF((40 - (40 - $BG$2)) &lt; 0, 0,(40 - (40 - $BG$2)) * D38)</f>
         <v>15.9375</v>
       </c>
@@ -8168,13 +8168,6 @@
       <c r="A39" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="4">
-        <v>41930.956790606797</v>
-      </c>
-      <c r="F39" s="5"/>
       <c r="G39" s="4">
         <f t="shared" ref="G39:AL39" si="17">SUM(G3:G38)</f>
         <v>47</v>
@@ -8392,13 +8385,6 @@
       <c r="A40" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="5">
-        <v>8776115.5432872735</v>
-      </c>
       <c r="G40" s="5">
         <f>SUM(B3*G3,B4*G4,B5*G5,B6*G6,B7*G7,B8*G8,B9*G9,B10*G10,B11*G11,B12*G12,B13*G13,B14*G14,B15*G15,B16*G16,B17*G17,B18*G18,B19*G19,B20*G20,B21*G21,B22*G22,B23*G23,B24*G24,B25*G25,B26*G26,B27*G27,B28*G28,B29*G29,B30*G30,B31*G31,B32*G32,B33*G33,B34*G34,B35*G35,B36*G36,B37*G37,B38*G38)</f>
         <v>9906</v>
@@ -8616,7 +8602,7 @@
       <c r="A41" t="s">
         <v>98</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="5">
         <v>8958790</v>
       </c>
     </row>
@@ -8624,7 +8610,19 @@
       <c r="A42" t="s">
         <v>99</v>
       </c>
-      <c r="E42">
+      <c r="B42" s="5">
+        <f>AVERAGE(B3:B38)</f>
+        <v>209.97222222222223</v>
+      </c>
+      <c r="C42" s="5">
+        <f>AVERAGE(C3:C38)</f>
+        <v>210.08571428571429</v>
+      </c>
+      <c r="D42" s="4">
+        <f>AVERAGE(D3:D38)</f>
+        <v>0.88278352904834845</v>
+      </c>
+      <c r="E42" s="4">
         <f>SUM(E3:E38)</f>
         <v>41930.956790606921</v>
       </c>
@@ -8662,6 +8660,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>